<commit_message>
add template cardio_index function
</commit_message>
<xml_diff>
--- a/sources/biomarker_reference.xlsx
+++ b/sources/biomarker_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\conig\repos\screentime_biomarkers\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB9537A-0220-4C70-AAC3-9F3802AEA98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E154D47B-4ABA-4779-846C-2D39035740EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="750" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>Age_years</t>
+  </si>
+  <si>
+    <t>Sex</t>
   </si>
 </sst>
 </file>
@@ -762,7 +762,7 @@
   <autoFilter ref="A1:Q29" xr:uid="{F501BE2B-99D8-4675-85E2-8D2EA0FB98EC}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{A10B96A6-FFC3-4C94-BD00-384C679F6DC0}" name="Variable" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{45E4C155-84FD-4426-B117-61539A97DFE3}" name="Gender" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{45E4C155-84FD-4426-B117-61539A97DFE3}" name="Sex" dataDxfId="15"/>
     <tableColumn id="3" xr3:uid="{076AD6DD-8B99-4F8C-927B-088BCD709E31}" name="Age_years" dataDxfId="14"/>
     <tableColumn id="4" xr3:uid="{8063D9A3-EA0D-487E-84FB-72B6CCC06196}" name="SBP (mmHg)" dataDxfId="13"/>
     <tableColumn id="5" xr3:uid="{1A7E8CB7-35E7-4763-8B50-10D408884E14}" name="DBP (mmHg)" dataDxfId="12"/>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,13 +1075,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -1131,7 +1131,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5">
         <v>6</v>
@@ -1184,7 +1184,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5">
         <v>7</v>
@@ -1237,7 +1237,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5">
         <v>8</v>
@@ -1290,7 +1290,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5">
         <v>9</v>
@@ -1343,7 +1343,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5">
         <v>10</v>
@@ -1396,7 +1396,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5">
         <v>11</v>
@@ -1449,7 +1449,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5">
         <v>12</v>
@@ -1502,7 +1502,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5">
         <v>13</v>
@@ -1555,7 +1555,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5">
         <v>14</v>
@@ -1608,7 +1608,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5">
         <v>15</v>
@@ -1661,7 +1661,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5">
         <v>16</v>
@@ -1714,7 +1714,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5">
         <v>17</v>
@@ -1767,7 +1767,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="5">
         <v>18</v>
@@ -1820,7 +1820,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>16</v>
@@ -1873,7 +1873,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="7">
         <v>6</v>
@@ -1926,7 +1926,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="8">
         <v>7</v>
@@ -1979,7 +1979,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="8">
         <v>8</v>
@@ -2032,7 +2032,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="8">
         <v>9</v>
@@ -2085,7 +2085,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="8">
         <v>10</v>
@@ -2138,7 +2138,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="8">
         <v>11</v>
@@ -2191,7 +2191,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="8">
         <v>12</v>
@@ -2244,7 +2244,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="8">
         <v>13</v>
@@ -2297,7 +2297,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="8">
         <v>14</v>
@@ -2350,7 +2350,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="8">
         <v>15</v>
@@ -2403,7 +2403,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="8">
         <v>16</v>
@@ -2456,7 +2456,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="8">
         <v>17</v>
@@ -2509,7 +2509,7 @@
         <v>14</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="8">
         <v>18</v>
@@ -2562,7 +2562,7 @@
         <v>15</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>16</v>
@@ -2628,7 +2628,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>